<commit_message>
excel dosyaları ve grafikler guncellendi
</commit_message>
<xml_diff>
--- a/2018.xlsx
+++ b/2018.xlsx
@@ -280,9 +280,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -429,36 +433,36 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="36.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="8.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -469,16 +473,16 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>20</v>
       </c>
     </row>
@@ -489,16 +493,16 @@
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>2348</v>
       </c>
     </row>
@@ -509,16 +513,16 @@
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>21</v>
       </c>
     </row>
@@ -529,16 +533,16 @@
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>165</v>
       </c>
     </row>
@@ -549,16 +553,16 @@
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>125</v>
       </c>
     </row>
@@ -569,16 +573,16 @@
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>6511</v>
       </c>
     </row>
@@ -589,16 +593,16 @@
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>23</v>
       </c>
     </row>
@@ -609,13 +613,13 @@
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <v>400</v>
       </c>
     </row>
@@ -626,16 +630,16 @@
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>1008</v>
       </c>
     </row>
@@ -646,16 +650,16 @@
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>85</v>
       </c>
     </row>
@@ -666,16 +670,16 @@
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <v>406</v>
       </c>
     </row>
@@ -686,16 +690,16 @@
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="4" t="n">
         <v>211</v>
       </c>
     </row>
@@ -706,16 +710,16 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>12</v>
       </c>
     </row>
@@ -726,13 +730,13 @@
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="4" t="n">
         <v>143</v>
       </c>
     </row>
@@ -743,13 +747,13 @@
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>200</v>
       </c>
     </row>
@@ -760,16 +764,16 @@
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="4" t="n">
         <v>11</v>
       </c>
     </row>
@@ -780,16 +784,16 @@
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="3" t="n">
+      <c r="F18" s="4" t="n">
         <v>10</v>
       </c>
     </row>
@@ -800,16 +804,16 @@
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="4" t="n">
         <v>7822</v>
       </c>
     </row>
@@ -820,16 +824,16 @@
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="4" t="n">
         <v>7555</v>
       </c>
     </row>
@@ -840,16 +844,16 @@
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -860,16 +864,16 @@
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>567</v>
       </c>
     </row>
@@ -880,16 +884,16 @@
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="4" t="n">
         <v>73</v>
       </c>
     </row>
@@ -900,16 +904,16 @@
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="4" t="n">
         <v>1156</v>
       </c>
     </row>
@@ -920,16 +924,16 @@
       <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="4" t="n">
         <v>165</v>
       </c>
     </row>
@@ -940,16 +944,16 @@
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="4" t="n">
         <v>703</v>
       </c>
     </row>
@@ -960,16 +964,16 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="4" t="n">
         <v>15</v>
       </c>
     </row>
@@ -980,16 +984,16 @@
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>85</v>
       </c>
     </row>
@@ -1000,13 +1004,13 @@
       <c r="B29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="4" t="n">
         <v>288</v>
       </c>
     </row>
@@ -1017,16 +1021,16 @@
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1037,16 +1041,16 @@
       <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>208</v>
       </c>
     </row>
@@ -1057,16 +1061,16 @@
       <c r="B32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="3" t="n">
+      <c r="F32" s="4" t="n">
         <v>390</v>
       </c>
     </row>
@@ -1077,16 +1081,16 @@
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="4" t="n">
         <v>186</v>
       </c>
     </row>
@@ -1097,13 +1101,13 @@
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F34" s="4" t="n">
         <v>65</v>
       </c>
     </row>
@@ -1114,16 +1118,16 @@
       <c r="B35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="3" t="n">
+      <c r="F35" s="4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1134,16 +1138,16 @@
       <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="F36" s="4" t="n">
         <v>180</v>
       </c>
     </row>
@@ -1154,16 +1158,16 @@
       <c r="B37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="4" t="n">
         <v>350</v>
       </c>
     </row>
@@ -1174,16 +1178,16 @@
       <c r="B38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" s="4" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1194,16 +1198,16 @@
       <c r="B39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1214,16 +1218,16 @@
       <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1234,13 +1238,13 @@
       <c r="B41" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="4" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1251,16 +1255,16 @@
       <c r="B42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1271,13 +1275,13 @@
       <c r="B43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="3" t="n">
+      <c r="F43" s="4" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1288,16 +1292,16 @@
       <c r="B44" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="3" t="n">
+      <c r="F44" s="4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1308,16 +1312,16 @@
       <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="3" t="n">
+      <c r="F45" s="4" t="n">
         <v>77</v>
       </c>
     </row>
@@ -1328,16 +1332,16 @@
       <c r="B46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F46" s="3" t="n">
+      <c r="F46" s="4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1348,16 +1352,16 @@
       <c r="B47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F47" s="3" t="n">
+      <c r="F47" s="4" t="n">
         <v>945</v>
       </c>
     </row>
@@ -1368,16 +1372,16 @@
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F48" s="4" t="n">
         <v>53</v>
       </c>
     </row>
@@ -1388,16 +1392,16 @@
       <c r="B49" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="3" t="n">
+      <c r="F49" s="4" t="n">
         <v>624</v>
       </c>
     </row>
@@ -1408,16 +1412,16 @@
       <c r="B50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F50" s="3" t="n">
+      <c r="F50" s="4" t="n">
         <v>240</v>
       </c>
     </row>
@@ -1428,16 +1432,16 @@
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="3" t="n">
+      <c r="F51" s="4" t="n">
         <v>77</v>
       </c>
     </row>
@@ -1448,16 +1452,16 @@
       <c r="B52" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F52" s="3" t="n">
+      <c r="F52" s="4" t="n">
         <v>163</v>
       </c>
     </row>
@@ -1468,16 +1472,16 @@
       <c r="B53" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="3" t="n">
+      <c r="F53" s="4" t="n">
         <v>375</v>
       </c>
     </row>
@@ -1488,16 +1492,16 @@
       <c r="B54" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="3" t="n">
+      <c r="F54" s="4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1508,16 +1512,16 @@
       <c r="B55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F55" s="3" t="n">
+      <c r="F55" s="4" t="n">
         <v>38</v>
       </c>
     </row>
@@ -1540,13 +1544,13 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D:D A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="1131.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>